<commit_message>
boxplots para la elowyn DONEEEEEEEEE
</commit_message>
<xml_diff>
--- a/GSD/GSD_box_plots/results/percentile_difference_summary.xlsx
+++ b/GSD/GSD_box_plots/results/percentile_difference_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\GSD_box_plots\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC2CC31-EE06-484F-BD3F-7FDC0A55AA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF71675C-BBA6-423E-88F1-7EC201EC587D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B2654242-1630-4848-886A-878F895EB92C}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{B2654242-1630-4848-886A-878F895EB92C}"/>
   </bookViews>
   <sheets>
     <sheet name="Original Sizes" sheetId="1" r:id="rId1"/>
@@ -192,7 +192,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -202,7 +202,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US">
+              <a:rPr lang="en-US" sz="1200">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -210,14 +210,14 @@
               <a:t>Water</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0">
+              <a:rPr lang="en-US" sz="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t> Column - Concentration Percentile Trends</a:t>
+              <a:t> Column - Concentration Percentile Trends - Original Sizes</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US">
+            <a:endParaRPr lang="en-US" sz="1200">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -238,7 +238,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -1069,7 +1069,7 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Sediment Trap - Percentile Differences (SM-SP)</a:t>
+              <a:t>Sediment Trap - Percentile Differences (SM-SP) - New Sizes</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1100">
               <a:solidFill>
@@ -1079,6 +1079,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11469811558679369"/>
+          <c:y val="2.6315789473684209E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1187,13 +1195,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-2.3931750000000109</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2.6852499999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.14704999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1267,13 +1275,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-4.4918499999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.2098</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.19890000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1347,13 +1355,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-6.7309999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.4710000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.25795000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1760,13 +1768,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-52.307886712647601</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>-40.319257649769149</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>-30.867145573277345</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1840,13 +1848,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-40.745929842342122</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>-33.203159886721863</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>-30.119172750000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1920,13 +1928,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-58.425597247631686</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>-26.273430274874684</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>-31.455074250000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2324,13 +2332,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-127.97289407777666</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>-30.142852112676064</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>-38.993537190082648</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2404,13 +2412,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-145.28754683376837</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>-30.86313186813187</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>-39.123554794520551</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2484,13 +2492,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-160.80781625961859</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>-34.679138817480712</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>-41.231011729790843</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2755,7 +2763,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -2765,7 +2773,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US">
+              <a:rPr lang="en-US" sz="1200">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -2773,14 +2781,14 @@
               <a:t>Sediment Traps </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0">
+              <a:rPr lang="en-US" sz="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>- Weight Percentile Trends</a:t>
+              <a:t>- Weight Percentile Trends - Original Sizes</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US">
+            <a:endParaRPr lang="en-US" sz="1200">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -2801,7 +2809,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -3640,7 +3648,7 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t> Column - Percentile Differences (SM-SP)</a:t>
+              <a:t> Column - Percentile Differences (SM-SP) - Original Sizes</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1100">
               <a:solidFill>
@@ -3736,16 +3744,19 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>'Original Sizes'!$A$14:$A$16</c:f>
+              <c:f>'Original Sizes'!$A$13:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>Coarse Sand</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Fine Sand</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Silt</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Clay</c:v>
                 </c:pt>
               </c:strCache>
@@ -3753,17 +3764,20 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Original Sizes'!$H$14:$H$16</c:f>
+              <c:f>'Original Sizes'!$H$13:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>0.95688195599999104</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>9.9022290682499996</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4.4180664942500005</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.35144205875000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -3816,16 +3830,19 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>'Original Sizes'!$A$14:$A$16</c:f>
+              <c:f>'Original Sizes'!$A$13:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>Coarse Sand</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Fine Sand</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Silt</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Clay</c:v>
                 </c:pt>
               </c:strCache>
@@ -3833,17 +3850,20 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Original Sizes'!$I$14:$I$16</c:f>
+              <c:f>'Original Sizes'!$I$13:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>1.2413300810000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>12.052429995499901</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>6.1313345855000003</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.44911781099999998</c:v>
                 </c:pt>
               </c:numCache>
@@ -3896,16 +3916,19 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>'Original Sizes'!$A$14:$A$16</c:f>
+              <c:f>'Original Sizes'!$A$13:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>Coarse Sand</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Fine Sand</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Silt</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Clay</c:v>
                 </c:pt>
               </c:strCache>
@@ -3913,17 +3936,20 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Original Sizes'!$J$14:$J$16</c:f>
+              <c:f>'Original Sizes'!$J$13:$J$16</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>1.8549177192499999</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>16.625548595000001</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>12.154502976749999</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.95534258949999995</c:v>
                 </c:pt>
               </c:numCache>
@@ -4205,7 +4231,7 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Sediment Trap - Percentile Differences (SM-SP)</a:t>
+              <a:t>Sediment Trap - Percentile Differences (SM-SP) - Original Sizes</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1100">
               <a:solidFill>
@@ -5904,7 +5930,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -5914,7 +5940,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US">
+              <a:rPr lang="en-US" sz="1200">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
@@ -5922,14 +5948,14 @@
               <a:t>Water</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0">
+              <a:rPr lang="en-US" sz="1200" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t> Column - Concentration Percentile Trends</a:t>
+              <a:t> Column - Concentration Percentile Trends - New Sizes</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US">
+            <a:endParaRPr lang="en-US" sz="1200">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -5950,7 +5976,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
@@ -6035,6 +6061,15 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="1">
+                  <c:v>3.2460896942500002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3720968172500001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.8925017750000003E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6101,6 +6136,15 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="1">
+                  <c:v>5.1774824810000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9881757034999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.122076691</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6167,6 +6211,15 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="1">
+                  <c:v>9.6481058797500001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.3097380212500003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1923304455</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6237,6 +6290,15 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="1">
+                  <c:v>5.605113974</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.1097737370000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18973258500000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6303,6 +6365,15 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="1">
+                  <c:v>10.16890712</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.227002969999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6369,6 +6440,15 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="1">
+                  <c:v>13.42753664</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.922344840000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6717,7 +6797,7 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>- Weight Percentile Trends</a:t>
+              <a:t>- Weight Percentile Trends - New Sizes</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
               <a:solidFill>
@@ -6825,6 +6905,18 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>13.760350000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.2619000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3972500000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.4950000000000007E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6891,6 +6983,18 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>17.811199999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.863</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7951999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12959999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6957,6 +7061,18 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>28.545749999999899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.2958</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3639999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18429999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -7027,6 +7143,18 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.01125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.8687249999999898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0824999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.24199999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -7093,6 +7221,18 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.71265</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.3711500000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0049999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.32850000000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -7159,6 +7299,18 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.6005750000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.5648</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.835</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.44224999999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -7507,7 +7659,7 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t> Column - Percentile Differences (SM-SP)</a:t>
+              <a:t> Column - Percentile Differences (SM-SP) - New Sizes</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1100">
               <a:solidFill>
@@ -7625,13 +7777,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2.3590242797499998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.7376769197500002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.13080756725000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7705,13 +7857,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>4.9914246389999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6.2388272664999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.27792330900000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7785,13 +7937,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>3.7794307602499995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>9.6126068187500007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.40766955449999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14989,12 +15141,8 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>CS</a:t>
-          </a:r>
-          <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>            FS               S                C</a:t>
+            <a:t> FS                     S                     C</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -15389,12 +15537,8 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>CS</a:t>
-          </a:r>
-          <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>            FS               S                C</a:t>
+            <a:t>  FS                     S                    C</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -15442,14 +15586,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>565589</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>52552</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>44669</xdr:rowOff>
+      <xdr:rowOff>85397</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>2299</xdr:colOff>
+      <xdr:colOff>291334</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>130394</xdr:rowOff>
     </xdr:to>
@@ -15466,8 +15610,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14767364" y="2711669"/>
-          <a:ext cx="1875110" cy="276225"/>
+          <a:off x="14885276" y="2752397"/>
+          <a:ext cx="2071524" cy="235497"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15498,12 +15642,8 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>CS</a:t>
-          </a:r>
-          <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>            FS               S                C</a:t>
+            <a:t>FS                   S                      C</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -16043,8 +16183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2800FBFC-ED83-41EB-8E42-FB801C25BE72}">
   <dimension ref="A2:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X36" sqref="X36"/>
+    <sheetView topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16607,8 +16747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{646353ED-E387-4441-9F2D-6062223C8CA0}">
   <dimension ref="A2:M16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16702,140 +16842,188 @@
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="B5" s="5">
+        <v>13.760350000000001</v>
+      </c>
+      <c r="C5" s="5">
+        <v>17.811199999999999</v>
+      </c>
+      <c r="D5" s="5">
+        <v>28.545749999999899</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1.01125</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1.71265</v>
+      </c>
+      <c r="G5" s="5">
+        <v>3.6005750000000001</v>
+      </c>
       <c r="H5" s="1">
         <f>E5-B5</f>
-        <v>0</v>
+        <v>-12.7491</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ref="I5:J8" si="0">F5-C5</f>
-        <v>0</v>
+        <v>-16.098549999999999</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K5" s="2" t="e">
+        <v>-24.9451749999999</v>
+      </c>
+      <c r="K5" s="2">
         <f>E5-B5/E5*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L5" s="2" t="e">
+        <v>-1359.7155732385661</v>
+      </c>
+      <c r="L5" s="2">
         <f t="shared" ref="L5:M8" si="1">F5-C5/F5*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M5" s="2" t="e">
+        <v>-1038.2663299433625</v>
+      </c>
+      <c r="M5" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>-789.21029548596118</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="B6" s="5">
+        <v>9.2619000000000007</v>
+      </c>
+      <c r="C6" s="5">
+        <v>12.863</v>
+      </c>
+      <c r="D6" s="5">
+        <v>16.2958</v>
+      </c>
+      <c r="E6" s="5">
+        <v>6.8687249999999898</v>
+      </c>
+      <c r="F6" s="5">
+        <v>8.3711500000000001</v>
+      </c>
+      <c r="G6" s="5">
+        <v>9.5648</v>
+      </c>
       <c r="H6" s="1">
         <f t="shared" ref="H6:H8" si="2">E6-B6</f>
-        <v>0</v>
+        <v>-2.3931750000000109</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-4.4918499999999995</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="2" t="e">
+        <v>-6.7309999999999999</v>
+      </c>
+      <c r="K6" s="2">
         <f t="shared" ref="K6:K8" si="3">E6-B6/E6*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L6" s="2" t="e">
+        <v>-127.97289407777666</v>
+      </c>
+      <c r="L6" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M6" s="2" t="e">
+        <v>-145.28754683376837</v>
+      </c>
+      <c r="M6" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>-160.80781625961859</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="B7" s="5">
+        <v>1.3972500000000001</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1.7951999999999999</v>
+      </c>
+      <c r="D7" s="5">
+        <v>2.3639999999999999</v>
+      </c>
+      <c r="E7" s="5">
+        <v>4.0824999999999996</v>
+      </c>
+      <c r="F7" s="5">
+        <v>5.0049999999999999</v>
+      </c>
+      <c r="G7" s="5">
+        <v>5.835</v>
+      </c>
       <c r="H7" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.6852499999999995</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.2098</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="2" t="e">
+        <v>3.4710000000000001</v>
+      </c>
+      <c r="K7" s="2">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L7" s="2" t="e">
+        <v>-30.142852112676064</v>
+      </c>
+      <c r="L7" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M7" s="2" t="e">
+        <v>-30.86313186813187</v>
+      </c>
+      <c r="M7" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>-34.679138817480712</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="B8" s="5">
+        <v>9.4950000000000007E-2</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.12959999999999999</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.18429999999999999</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.32850000000000001</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.44224999999999998</v>
+      </c>
       <c r="H8" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.14704999999999999</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.19890000000000002</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K8" s="2" t="e">
+        <v>0.25795000000000001</v>
+      </c>
+      <c r="K8" s="2">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L8" s="2" t="e">
+        <v>-38.993537190082648</v>
+      </c>
+      <c r="L8" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M8" s="2" t="e">
+        <v>-39.123554794520551</v>
+      </c>
+      <c r="M8" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>-41.231011729790843</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -16952,105 +17140,141 @@
       <c r="A14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="B14" s="5">
+        <v>3.2460896942500002</v>
+      </c>
+      <c r="C14" s="5">
+        <v>5.1774824810000002</v>
+      </c>
+      <c r="D14" s="5">
+        <v>9.6481058797500001</v>
+      </c>
+      <c r="E14" s="6">
+        <v>5.605113974</v>
+      </c>
+      <c r="F14" s="6">
+        <v>10.16890712</v>
+      </c>
+      <c r="G14" s="6">
+        <v>13.42753664</v>
+      </c>
       <c r="H14" s="1">
         <f>E14-B14</f>
-        <v>0</v>
+        <v>2.3590242797499998</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4.9914246389999999</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="2" t="e">
+        <v>3.7794307602499995</v>
+      </c>
+      <c r="K14" s="2">
         <f t="shared" ref="K14:K16" si="6">E14-B14/E14*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L14" s="2" t="e">
+        <v>-52.307886712647601</v>
+      </c>
+      <c r="L14" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M14" s="2" t="e">
+        <v>-40.745929842342122</v>
+      </c>
+      <c r="M14" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>-58.425597247631686</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="B15" s="5">
+        <v>3.3720968172500001</v>
+      </c>
+      <c r="C15" s="5">
+        <v>4.9881757034999996</v>
+      </c>
+      <c r="D15" s="5">
+        <v>7.3097380212500003</v>
+      </c>
+      <c r="E15" s="6">
+        <v>7.1097737370000003</v>
+      </c>
+      <c r="F15" s="6">
+        <v>11.227002969999999</v>
+      </c>
+      <c r="G15" s="6">
+        <v>16.922344840000001</v>
+      </c>
       <c r="H15" s="1">
         <f>E15-B15</f>
-        <v>0</v>
+        <v>3.7376769197500002</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.2388272664999995</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K15" s="2" t="e">
+        <v>9.6126068187500007</v>
+      </c>
+      <c r="K15" s="2">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L15" s="2" t="e">
+        <v>-40.319257649769149</v>
+      </c>
+      <c r="L15" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M15" s="2" t="e">
+        <v>-33.203159886721863</v>
+      </c>
+      <c r="M15" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>-26.273430274874684</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="B16" s="5">
+        <v>5.8925017750000003E-2</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0.122076691</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0.1923304455</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0.18973258500000001</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0.6</v>
+      </c>
       <c r="H16" s="1">
         <f>E16-B16</f>
-        <v>0</v>
+        <v>0.13080756725000001</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.27792330900000001</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="2" t="e">
+        <v>0.40766955449999998</v>
+      </c>
+      <c r="K16" s="2">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L16" s="2" t="e">
+        <v>-30.867145573277345</v>
+      </c>
+      <c r="L16" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M16" s="2" t="e">
+        <v>-30.119172750000004</v>
+      </c>
+      <c r="M16" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>-31.455074250000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>